<commit_message>
new enrichment physio aging
</commit_message>
<xml_diff>
--- a/_05_Enrichment_PhysioAging_Genes/output_tables/enrichment_details/enrichment_physioaging.xlsx
+++ b/_05_Enrichment_PhysioAging_Genes/output_tables/enrichment_details/enrichment_physioaging.xlsx
@@ -87,7 +87,7 @@
     <t>Breast down-reg. genes</t>
   </si>
   <si>
-    <t>{'TERT', 'RAD51', 'ATM', 'TP53', 'ERCC1', 'ERCC8', 'CDKN1A', 'ERCC2', 'AKT1', 'ATR', 'WRN', 'BRCA1', 'XRCC5', 'PTEN', 'CDK7', 'LMNA', 'POLA1', 'RAD52'}</t>
+    <t>{'ERCC1', 'CDK7', 'TERT', 'RAD52', 'XRCC5', 'LMNA', 'RAD51', 'AKT1', 'PTEN', 'ATR', 'POLA1', 'ERCC2', 'CDKN1A', 'ATM', 'WRN', 'TP53', 'ERCC8', 'BRCA1'}</t>
   </si>
   <si>
     <t>{'DDB2'}</t>
@@ -96,28 +96,28 @@
     <t>{'ATM'}</t>
   </si>
   <si>
-    <t>{'AR', 'TERF1', 'APOO', 'ZMPSTE24', 'RAD51D'}</t>
-  </si>
-  <si>
-    <t>{'NEIL1', 'DVL2', 'DVL1', 'MCM7', 'TDP1', 'DAXX', 'RAD9A', 'LIG1', 'POLE'}</t>
-  </si>
-  <si>
-    <t>{'RBBP8', 'CDK2', 'CDKN1A', 'DCLRE1C', 'HADHB'}</t>
-  </si>
-  <si>
-    <t>{'ATRX', 'USP12', 'RAD51C', 'RAD50', 'CTNNB1', 'TP53BP1', 'MCM4', 'DCP2', 'CCND2'}</t>
-  </si>
-  <si>
-    <t>{'CDKN1A', 'CUL4A', 'USP1', 'SUMO2', 'XRCC6'}</t>
-  </si>
-  <si>
-    <t>{'AR', 'MTX2', 'CHCHD10', 'CDK2', 'SAMM50'}</t>
-  </si>
-  <si>
-    <t>{'CCNH', 'MDM4', 'USP34'}</t>
-  </si>
-  <si>
-    <t>{'POLD1', 'DVL2', 'CTNNB1', 'TP53', 'KDM1A', 'RAD9A', 'RTEL1'}</t>
+    <t>{'APOO', 'AR', 'TERF1', 'RAD51D', 'ZMPSTE24'}</t>
+  </si>
+  <si>
+    <t>{'TDP1', 'RAD9A', 'NEIL1', 'LIG1', 'POLE', 'DVL1', 'DVL2', 'DAXX', 'MCM7'}</t>
+  </si>
+  <si>
+    <t>{'DCLRE1C', 'RBBP8', 'CDKN1A', 'HADHB', 'CDK2'}</t>
+  </si>
+  <si>
+    <t>{'MCM4', 'RAD51C', 'RAD50', 'TP53BP1', 'DCP2', 'CCND2', 'USP12', 'CTNNB1', 'ATRX'}</t>
+  </si>
+  <si>
+    <t>{'XRCC6', 'CUL4A', 'SUMO2', 'CDKN1A', 'USP1'}</t>
+  </si>
+  <si>
+    <t>{'MTX2', 'AR', 'SAMM50', 'CDK2', 'CHCHD10'}</t>
+  </si>
+  <si>
+    <t>{'MDM4', 'USP34', 'CCNH'}</t>
+  </si>
+  <si>
+    <t>{'RAD9A', 'POLD1', 'KDM1A', 'CTNNB1', 'DVL2', 'TP53', 'RTEL1'}</t>
   </si>
   <si>
     <t>['TERT', 'ATM', 'ERCC2', 'ERCC8', 'WRN', 'LMNA', 'PTEN', 'ERCC1', 'ATR']</t>
@@ -144,7 +144,7 @@
     <t>cluster_3</t>
   </si>
   <si>
-    <t>{'NCOR2', 'PML', 'TFDP1', 'CDKN2B', 'E2F1', 'TP53', 'RB1', 'CDKN1A', 'FOXO3', 'CDKN2A', 'AKT1', 'ERCC2', 'BRCA1', 'FOXO1', 'CDK7', 'SIRT1'}</t>
+    <t>{'RB1', 'CDK7', 'AKT1', 'PML', 'SIRT1', 'TFDP1', 'FOXO1', 'FOXO3', 'E2F1', 'ERCC2', 'CDKN1A', 'CDKN2B', 'TP53', 'CDKN2A', 'BRCA1', 'NCOR2'}</t>
   </si>
   <si>
     <t>{'CDKN2A'}</t>
@@ -153,28 +153,28 @@
     <t>{'MAML2', 'E2F5'}</t>
   </si>
   <si>
-    <t>{'THRB', 'WWTR1', 'TEAD1', 'FOXO3', 'RBPJ', 'FOXO1', 'AMOTL2', 'ESR1', 'AR', 'CDH10', 'MAML2', 'AMOT', 'UBE2J1', 'ZFPM2', 'APH1B', 'TBX5', 'ERLEC1', 'ARHGAP26', 'ELK3'}</t>
-  </si>
-  <si>
-    <t>{'VDR', 'HDAC10', 'EGR2', 'CDKN2D', 'KAT2A', 'BRF1', 'RXRB', 'DAXX', 'GTF3C1', 'GTF2H4'}</t>
-  </si>
-  <si>
-    <t>{'NOTCH2', 'YAP1', 'SIRT1', 'MAML2', 'STAT3', 'CDKN1A', 'CDKN2A', 'EGFR', 'BOC', 'CDK2', 'CBFB', 'SMAD1', 'PKN3', 'SOX9'}</t>
-  </si>
-  <si>
-    <t>{'THRB', 'RANGAP1', 'CTNNB1', 'RXRB', 'SRC', 'SMAD3', 'GTF2H1', 'CCND2', 'SMARCA2'}</t>
-  </si>
-  <si>
-    <t>{'SMAD4', 'PIK3R1', 'ADAM10', 'SNW1', 'CTNNA1', 'CDKN1A', 'FOXO3', 'RBPJ', 'FOXO1', 'CREBBP', 'SIRT1', 'SUMO2', 'CCNT1'}</t>
-  </si>
-  <si>
-    <t>{'AR', 'PML', 'HIVEP3', 'CDKN2C', 'CDK2'}</t>
-  </si>
-  <si>
-    <t>{'MAF', 'CCNH', 'SEL1L', 'CDKN2A'}</t>
-  </si>
-  <si>
-    <t>{'VGLL4', 'JUP', 'CTNNB1', 'TP53', 'SMARCA4', 'KDM1A', 'TGIF1', 'SMARCC2', 'ELK1', 'SMARCB1', 'MED12'}</t>
+    <t>{'FOXO1', 'FOXO3', 'TEAD1', 'TBX5', 'MAML2', 'ERLEC1', 'WWTR1', 'AMOTL2', 'ELK3', 'RBPJ', 'APH1B', 'ARHGAP26', 'CDH10', 'ZFPM2', 'UBE2J1', 'AMOT', 'THRB', 'ESR1', 'AR'}</t>
+  </si>
+  <si>
+    <t>{'GTF3C1', 'BRF1', 'CDKN2D', 'KAT2A', 'VDR', 'RXRB', 'EGR2', 'GTF2H4', 'DAXX', 'HDAC10'}</t>
+  </si>
+  <si>
+    <t>{'MAML2', 'NOTCH2', 'YAP1', 'EGFR', 'SOX9', 'PKN3', 'SIRT1', 'CBFB', 'STAT3', 'CDKN1A', 'SMAD1', 'CDK2', 'BOC', 'CDKN2A'}</t>
+  </si>
+  <si>
+    <t>{'GTF2H1', 'SMAD3', 'THRB', 'SMARCA2', 'RXRB', 'CCND2', 'CTNNB1', 'RANGAP1', 'SRC'}</t>
+  </si>
+  <si>
+    <t>{'SMAD4', 'RBPJ', 'SNW1', 'CREBBP', 'ADAM10', 'SIRT1', 'FOXO1', 'SUMO2', 'PIK3R1', 'FOXO3', 'CDKN1A', 'CTNNA1', 'CCNT1'}</t>
+  </si>
+  <si>
+    <t>{'AR', 'PML', 'CDK2', 'CDKN2C', 'HIVEP3'}</t>
+  </si>
+  <si>
+    <t>{'CDKN2A', 'MAF', 'CCNH', 'SEL1L'}</t>
+  </si>
+  <si>
+    <t>{'SMARCA4', 'ELK1', 'MED12', 'TGIF1', 'SMARCB1', 'SMARCC2', 'KDM1A', 'CTNNB1', 'TP53', 'JUP', 'VGLL4'}</t>
   </si>
   <si>
     <t>['ERCC2']</t>
@@ -186,37 +186,37 @@
     <t>cluster_5</t>
   </si>
   <si>
-    <t>{'PIK3CB', 'IRS1', 'HRAS', 'INSR', 'CDC42', 'ELN', 'HTRA2', 'IGF1R', 'SHC1'}</t>
-  </si>
-  <si>
-    <t>{'PDGFB', 'PAPSS2', 'SYTL3', 'RET'}</t>
-  </si>
-  <si>
-    <t>{'MS4A1', 'PYCR1', 'CR2', 'FBLN2'}</t>
-  </si>
-  <si>
-    <t>{'AOX1', 'GPX8', 'IRS1', 'C3', 'MFAP5', 'FYN', 'SIRPA', 'PDGFRA', 'DLC1', 'TGFBR1', 'GPX7', 'MSR1', 'KIF5B', 'CXCL12', 'CYCS', 'CYS1', 'EDN3', 'JAM3', 'FBLN5', 'ESR1', 'FBN1', 'ABL2', 'RHOJ', 'HSP90AA1', 'MFAP4', 'PIK3AP1', 'UACA', 'RHOQ', 'ITGA1', 'RPGRIP1L', 'NRP1', 'RHOA', 'PDGFRB', 'CERS6', 'DOCK4', 'COL5A2', 'GALNT12', 'PTK2', 'EMILIN1', 'RCN1', 'ANKS6', 'ELN', 'WIPF1', 'LTBP1', 'PIK3R3', 'ITGA9', 'THBS1', 'SH3KBP1', 'ITGAV', 'LOX', 'ADAMTS2'}</t>
-  </si>
-  <si>
-    <t>{'HGS', 'COL2A1', 'GRB7', 'TROAP', 'PSAT1', 'DVL2', 'CNKSR1', 'PIK3R2', 'GJB6', 'EPHB3', 'SEMA4D', 'PLK1', 'MOGS', 'COCH', 'ITGB7', 'PLXNB1', 'PLEKHH3', 'ADAM15'}</t>
-  </si>
-  <si>
-    <t>{'HGF', 'C3', 'FYN', 'PAPSS2', 'SYK', 'SERPINA1', 'CD44', 'TGFBR1', 'PARD3', 'MSR1', 'EGFR', 'LRP4', 'SHC1', 'TLN1', 'ECE1', 'PKN3', 'ITSN1', 'CD2AP', 'PIK3AP1', 'P4HA1', 'RHOQ', 'ITGB1', 'LCP2', 'ITGB5', 'TGFB1', 'FGG', 'SPP1', 'RAB27A', 'DOCK4', 'TGFB3', 'FLT1', 'FCGR1A', 'PXN', 'RANBP3L', 'LTBP1', 'ITGAV', 'CD81'}</t>
-  </si>
-  <si>
-    <t>{'DLGAP1', 'SOS1', 'AGPAT1', 'RCN2', 'SMAD3', 'AKAP10', 'CHRNA7', 'EPHA5', 'CTNNB1', 'DOCK3', 'SRC', 'F11R', 'DLG2', 'MET', 'PIK3CB', 'YWHAB', 'MYO5A', 'GOPC', 'DLG1'}</t>
-  </si>
-  <si>
-    <t>{'PIK3R1', 'XIAP', 'SMARCA5', 'YWHAB', 'COL4A5', 'COL4A3', 'LRCH3', 'KRAS', 'YWHAZ', 'EIF4H', 'SLC44A2'}</t>
-  </si>
-  <si>
-    <t>{'EML4', 'ALKBH7', 'AGPAT1', 'VEGFC', 'PARD6A', 'PDGFB'}</t>
-  </si>
-  <si>
-    <t>{'GPX8', 'XIAP', 'KITLG', 'OSTF1', 'DLC1', 'YWHAZ', 'MFAP4', 'RHOQ', 'MITF', 'TFRC', 'MYO5A', 'EML1'}</t>
-  </si>
-  <si>
-    <t>{'PARD6G', 'GTF2IRD1', 'DVL2', 'CTNNB1', 'AGRN', 'UNC119B', 'EPHB4', 'SHC1', 'ITGA3', 'PLXNB1', 'MED12'}</t>
+    <t>{'CDC42', 'HRAS', 'IGF1R', 'ELN', 'INSR', 'HTRA2', 'IRS1', 'SHC1', 'PIK3CB'}</t>
+  </si>
+  <si>
+    <t>{'PAPSS2', 'RET', 'PDGFB', 'SYTL3'}</t>
+  </si>
+  <si>
+    <t>{'FBLN2', 'CR2', 'MS4A1', 'PYCR1'}</t>
+  </si>
+  <si>
+    <t>{'RCN1', 'COL5A2', 'AOX1', 'LOX', 'PIK3R3', 'PTK2', 'GPX7', 'EDN3', 'PDGFRA', 'CYCS', 'PDGFRB', 'IRS1', 'CERS6', 'CYS1', 'EMILIN1', 'KIF5B', 'THBS1', 'FYN', 'DLC1', 'RPGRIP1L', 'ITGA1', 'C3', 'UACA', 'MFAP5', 'ADAMTS2', 'ABL2', 'LTBP1', 'SIRPA', 'CXCL12', 'JAM3', 'HSP90AA1', 'RHOA', 'FBN1', 'ELN', 'RHOJ', 'SH3KBP1', 'ITGA9', 'MSR1', 'WIPF1', 'MFAP4', 'GPX8', 'ESR1', 'ANKS6', 'NRP1', 'GALNT12', 'TGFBR1', 'FBLN5', 'DOCK4', 'RHOQ', 'ITGAV', 'PIK3AP1'}</t>
+  </si>
+  <si>
+    <t>{'ITGB7', 'GRB7', 'SEMA4D', 'MOGS', 'DVL2', 'EPHB3', 'PLK1', 'COL2A1', 'CNKSR1', 'PLEKHH3', 'GJB6', 'PIK3R2', 'PSAT1', 'TROAP', 'COCH', 'PLXNB1', 'HGS', 'ADAM15'}</t>
+  </si>
+  <si>
+    <t>{'HGF', 'SERPINA1', 'LCP2', 'CD2AP', 'P4HA1', 'FGG', 'EGFR', 'FYN', 'PKN3', 'TGFB1', 'C3', 'RAB27A', 'PAPSS2', 'LTBP1', 'ITSN1', 'LRP4', 'ITGB1', 'RANBP3L', 'FCGR1A', 'CD44', 'MSR1', 'SHC1', 'TLN1', 'FLT1', 'PARD3', 'TGFB3', 'CD81', 'SYK', 'TGFBR1', 'SPP1', 'DOCK4', 'ITGB5', 'PXN', 'RHOQ', 'ECE1', 'ITGAV', 'PIK3AP1'}</t>
+  </si>
+  <si>
+    <t>{'SOS1', 'MET', 'DLG2', 'SRC', 'PIK3CB', 'DOCK3', 'F11R', 'DLG1', 'CTNNB1', 'EPHA5', 'YWHAB', 'CHRNA7', 'GOPC', 'AGPAT1', 'MYO5A', 'RCN2', 'AKAP10', 'DLGAP1', 'SMAD3'}</t>
+  </si>
+  <si>
+    <t>{'SLC44A2', 'YWHAZ', 'LRCH3', 'KRAS', 'XIAP', 'COL4A3', 'SMARCA5', 'COL4A5', 'PIK3R1', 'EIF4H', 'YWHAB'}</t>
+  </si>
+  <si>
+    <t>{'AGPAT1', 'PARD6A', 'PDGFB', 'VEGFC', 'ALKBH7', 'EML4'}</t>
+  </si>
+  <si>
+    <t>{'MFAP4', 'MYO5A', 'YWHAZ', 'GPX8', 'MITF', 'KITLG', 'DLC1', 'EML1', 'XIAP', 'RHOQ', 'OSTF1', 'TFRC'}</t>
+  </si>
+  <si>
+    <t>{'EPHB4', 'MED12', 'PARD6G', 'UNC119B', 'AGRN', 'CTNNB1', 'DVL2', 'GTF2IRD1', 'PLXNB1', 'SHC1', 'ITGA3'}</t>
   </si>
   <si>
     <t>['INSR', 'ELN']</t>
@@ -243,7 +243,7 @@
     <t>cluster_4</t>
   </si>
   <si>
-    <t>{'IKBKB', 'HSPA1A', 'TP53', 'FOXO3', 'AKT1', 'NFKBIA', 'HTT'}</t>
+    <t>{'NFKBIA', 'HTT', 'HSPA1A', 'AKT1', 'FOXO3', 'IKBKB', 'TP53'}</t>
   </si>
   <si>
     <t>{'FADD'}</t>
@@ -252,19 +252,19 @@
     <t>{'RHPN2'}</t>
   </si>
   <si>
-    <t>{'CD14', 'IRAK3', 'HSP90AA1', 'FOXO3', 'CASP10', 'BCL2', 'TLR4', 'RAB8B', 'FKBP5', 'CFLAR'}</t>
-  </si>
-  <si>
-    <t>{'IKBKB', 'TBC1D17', 'LRSAM1', 'TAB1', 'NFKB2', 'IKBKE', 'NLRP1'}</t>
-  </si>
-  <si>
-    <t>{'CD14', 'BCL2L11', 'MCL1', 'MAP3K8', 'CASP1', 'LTBR', 'MYD88', 'TNFRSF1B', 'SFN', 'BCL2', 'TLR4', 'TNFRSF1A', 'NFKBIA', 'FKBP5', 'SHMT1', 'RELA', 'TNIP2'}</t>
+    <t>{'CD14', 'CFLAR', 'IRAK3', 'HSP90AA1', 'RAB8B', 'CASP10', 'BCL2', 'FOXO3', 'TLR4', 'FKBP5'}</t>
+  </si>
+  <si>
+    <t>{'NFKB2', 'NLRP1', 'TBC1D17', 'IKBKE', 'TAB1', 'IKBKB', 'LRSAM1'}</t>
+  </si>
+  <si>
+    <t>{'CASP1', 'NFKBIA', 'CD14', 'BCL2L11', 'TNIP2', 'TNFRSF1B', 'RELA', 'SHMT1', 'SFN', 'BCL2', 'LTBR', 'MCL1', 'FKBP5', 'TLR4', 'TNFRSF1A', 'MAP3K8', 'MYD88'}</t>
   </si>
   <si>
     <t>{'HSPH1', 'BAD', 'SARM1'}</t>
   </si>
   <si>
-    <t>{'FOXO3', 'CUL4A', 'CREBBP'}</t>
+    <t>{'CUL4A', 'CREBBP', 'FOXO3'}</t>
   </si>
   <si>
     <t>{'TICAM2'}</t>
@@ -273,43 +273,43 @@
     <t>{'CFLAR', 'CASP10', 'TLR4', 'IRAK3'}</t>
   </si>
   <si>
-    <t>{'TP53', 'SHMT2', 'TRAF2', 'FADD'}</t>
+    <t>{'SHMT2', 'TP53', 'FADD', 'TRAF2'}</t>
   </si>
   <si>
     <t>cluster_2</t>
   </si>
   <si>
-    <t>{'CDKN2B', 'E2F1', 'TP53', 'RB1', 'ERCC8', 'CDKN1A', 'FOXO3', 'CDKN2A', 'AKT1', 'MYC', 'FOXO1', 'CDK7', 'TFDP1'}</t>
-  </si>
-  <si>
-    <t>{'CDKN2A', 'SYTL3', 'DDB2'}</t>
+    <t>{'RB1', 'CDK7', 'AKT1', 'TFDP1', 'FOXO1', 'MYC', 'FOXO3', 'E2F1', 'CDKN1A', 'CDKN2B', 'TP53', 'ERCC8', 'CDKN2A'}</t>
+  </si>
+  <si>
+    <t>{'DDB2', 'CDKN2A', 'SYTL3'}</t>
   </si>
   <si>
     <t>{'E2F5', 'SUZ12'}</t>
   </si>
   <si>
-    <t>{'ESR1', 'AR', 'NQO1', 'YAF2', 'FOXO3', 'KIF5B', 'FOXO1'}</t>
+    <t>{'NQO1', 'AR', 'ESR1', 'KIF5B', 'FOXO1', 'FOXO3', 'YAF2'}</t>
   </si>
   <si>
     <t>{'KCTD15', 'CDKN2D', 'MCM7'}</t>
   </si>
   <si>
-    <t>{'GMNN', 'CDKN1A', 'CDKN2A', 'RAB27A', 'CDK2', 'SMAD1', 'STAT3'}</t>
-  </si>
-  <si>
-    <t>{'CDC6', 'OAZ2', 'CTNNB1', 'YAF2', 'YY1', 'KCTD1', 'SMAD3', 'MCM4', 'CCND2', 'MYO5A'}</t>
-  </si>
-  <si>
-    <t>{'SMAD4', 'PHC3', 'EPC1', 'YY1', 'CDKN1A', 'FOXO3', 'EHMT1', 'CUL4A', 'FOXO1', 'CREBBP'}</t>
-  </si>
-  <si>
-    <t>{'CITED4', 'AR', 'CDK2', 'CDKN2C'}</t>
-  </si>
-  <si>
-    <t>{'CDKN2A', 'CCNH', 'MYO5A'}</t>
-  </si>
-  <si>
-    <t>{'CITED4', 'CTNNB1', 'TP53', 'SMARCA4', 'KDM1A', 'TGIF1', 'EHMT2', 'PHC1'}</t>
+    <t>{'GMNN', 'STAT3', 'CDKN1A', 'SMAD1', 'RAB27A', 'CDK2', 'CDKN2A'}</t>
+  </si>
+  <si>
+    <t>{'MYO5A', 'MCM4', 'OAZ2', 'YY1', 'CDC6', 'KCTD1', 'CCND2', 'CTNNB1', 'SMAD3', 'YAF2'}</t>
+  </si>
+  <si>
+    <t>{'SMAD4', 'PHC3', 'YY1', 'CREBBP', 'CUL4A', 'FOXO1', 'FOXO3', 'EPC1', 'CDKN1A', 'EHMT1'}</t>
+  </si>
+  <si>
+    <t>{'AR', 'CDK2', 'CDKN2C', 'CITED4'}</t>
+  </si>
+  <si>
+    <t>{'MYO5A', 'CCNH', 'CDKN2A'}</t>
+  </si>
+  <si>
+    <t>{'EHMT2', 'PHC1', 'SMARCA4', 'TGIF1', 'KDM1A', 'CTNNB1', 'TP53', 'CITED4'}</t>
   </si>
   <si>
     <t>['ERCC8']</t>
@@ -330,31 +330,31 @@
     <t>{'HTT'}</t>
   </si>
   <si>
-    <t>{'CHML', 'PAWR', 'NT5E'}</t>
-  </si>
-  <si>
-    <t>{'NT5E', 'SALL1', 'LONRF3', 'ABCD2', 'OSBPL1A', 'ARHGDIG', 'PEX19', 'APH1B', 'RAB8B', 'PRKRA', 'PTP4A2', 'RAB32', 'RABEP1'}</t>
-  </si>
-  <si>
-    <t>{'TBC1D17', 'SLC6A8', 'C19orf54', 'SIRT2', 'TMEM102', 'PPFIA3', 'S1PR5', 'RAB38', 'GGA1'}</t>
-  </si>
-  <si>
-    <t>{'SLC6A8', 'PAWR', 'RAB34', 'ZFP36', 'RAB31', 'RAB13', 'USP3', 'TRIM4'}</t>
-  </si>
-  <si>
-    <t>{'RAB35', 'VAMP2', 'ABCD2', 'OSBPL1A', 'TMEM9', 'RAB14', 'CHM', 'PRKRA', 'RAB1A', 'BACE1', 'RABEP1'}</t>
-  </si>
-  <si>
-    <t>{'DICER1', 'ZFP36', 'CHM', 'RAB10', 'PRKRA'}</t>
-  </si>
-  <si>
-    <t>{'EHD3', 'C19orf54', 'GGA3', 'TMEM9'}</t>
-  </si>
-  <si>
-    <t>{'RAB31', 'NT5E', 'RAB3GAP1'}</t>
-  </si>
-  <si>
-    <t>{'TMEM102', 'PPFIA3', 'MICALL1'}</t>
+    <t>{'NT5E', 'CHML', 'PAWR'}</t>
+  </si>
+  <si>
+    <t>{'RABEP1', 'OSBPL1A', 'RAB32', 'RAB8B', 'ABCD2', 'APH1B', 'SALL1', 'PEX19', 'PTP4A2', 'ARHGDIG', 'NT5E', 'PRKRA', 'LONRF3'}</t>
+  </si>
+  <si>
+    <t>{'SLC6A8', 'C19orf54', 'TMEM102', 'S1PR5', 'PPFIA3', 'TBC1D17', 'SIRT2', 'RAB38', 'GGA1'}</t>
+  </si>
+  <si>
+    <t>{'SLC6A8', 'TRIM4', 'RAB34', 'ZFP36', 'USP3', 'RAB13', 'PAWR', 'RAB31'}</t>
+  </si>
+  <si>
+    <t>{'RAB35', 'CHM', 'RAB14', 'RABEP1', 'OSBPL1A', 'ABCD2', 'VAMP2', 'TMEM9', 'BACE1', 'PRKRA', 'RAB1A'}</t>
+  </si>
+  <si>
+    <t>{'DICER1', 'CHM', 'RAB10', 'ZFP36', 'PRKRA'}</t>
+  </si>
+  <si>
+    <t>{'GGA3', 'TMEM9', 'C19orf54', 'EHD3'}</t>
+  </si>
+  <si>
+    <t>{'NT5E', 'RAB3GAP1', 'RAB31'}</t>
+  </si>
+  <si>
+    <t>{'MICALL1', 'TMEM102', 'PPFIA3'}</t>
   </si>
   <si>
     <t>['RAB3GAP1']</t>

</xml_diff>

<commit_message>
fix bug in parsing seeds file
</commit_message>
<xml_diff>
--- a/_05_Enrichment_PhysioAging_Genes/output_tables/enrichment_details/enrichment_physioaging.xlsx
+++ b/_05_Enrichment_PhysioAging_Genes/output_tables/enrichment_details/enrichment_physioaging.xlsx
@@ -87,7 +87,7 @@
     <t>Breast down-reg. genes</t>
   </si>
   <si>
-    <t>{'ERCC1', 'CDK7', 'TERT', 'RAD52', 'XRCC5', 'LMNA', 'RAD51', 'AKT1', 'PTEN', 'ATR', 'POLA1', 'ERCC2', 'CDKN1A', 'ATM', 'WRN', 'TP53', 'ERCC8', 'BRCA1'}</t>
+    <t>{'TP53', 'CDKN1A', 'PTEN', 'TERT', 'BRCA1', 'ERCC2', 'ERCC1', 'ERCC8', 'ATM', 'POLA1', 'RAD52', 'XRCC5', 'CDK7', 'ATR', 'RAD51', 'LMNA', 'AKT1', 'WRN'}</t>
   </si>
   <si>
     <t>{'DDB2'}</t>
@@ -96,28 +96,28 @@
     <t>{'ATM'}</t>
   </si>
   <si>
-    <t>{'APOO', 'AR', 'TERF1', 'RAD51D', 'ZMPSTE24'}</t>
-  </si>
-  <si>
-    <t>{'TDP1', 'RAD9A', 'NEIL1', 'LIG1', 'POLE', 'DVL1', 'DVL2', 'DAXX', 'MCM7'}</t>
-  </si>
-  <si>
-    <t>{'DCLRE1C', 'RBBP8', 'CDKN1A', 'HADHB', 'CDK2'}</t>
-  </si>
-  <si>
-    <t>{'MCM4', 'RAD51C', 'RAD50', 'TP53BP1', 'DCP2', 'CCND2', 'USP12', 'CTNNB1', 'ATRX'}</t>
-  </si>
-  <si>
-    <t>{'XRCC6', 'CUL4A', 'SUMO2', 'CDKN1A', 'USP1'}</t>
-  </si>
-  <si>
-    <t>{'MTX2', 'AR', 'SAMM50', 'CDK2', 'CHCHD10'}</t>
-  </si>
-  <si>
-    <t>{'MDM4', 'USP34', 'CCNH'}</t>
-  </si>
-  <si>
-    <t>{'RAD9A', 'POLD1', 'KDM1A', 'CTNNB1', 'DVL2', 'TP53', 'RTEL1'}</t>
+    <t>{'ZMPSTE24', 'AR', 'TERF1', 'APOO', 'RAD51D'}</t>
+  </si>
+  <si>
+    <t>{'TDP1', 'DVL2', 'DAXX', 'LIG1', 'MCM7', 'NEIL1', 'POLE', 'RAD9A', 'DVL1'}</t>
+  </si>
+  <si>
+    <t>{'CDKN1A', 'DCLRE1C', 'CDK2', 'RBBP8', 'HADHB'}</t>
+  </si>
+  <si>
+    <t>{'MCM4', 'RAD50', 'RAD51C', 'ATRX', 'CTNNB1', 'DCP2', 'TP53BP1', 'CCND2', 'USP12'}</t>
+  </si>
+  <si>
+    <t>{'CDKN1A', 'USP1', 'SUMO2', 'CUL4A', 'XRCC6'}</t>
+  </si>
+  <si>
+    <t>{'AR', 'CDK2', 'SAMM50', 'CHCHD10', 'MTX2'}</t>
+  </si>
+  <si>
+    <t>{'USP34', 'MDM4', 'CCNH'}</t>
+  </si>
+  <si>
+    <t>{'TP53', 'RTEL1', 'DVL2', 'KDM1A', 'CTNNB1', 'POLD1', 'RAD9A'}</t>
   </si>
   <si>
     <t>['TERT', 'ATM', 'ERCC2', 'ERCC8', 'WRN', 'LMNA', 'PTEN', 'ERCC1', 'ATR']</t>
@@ -144,7 +144,7 @@
     <t>cluster_3</t>
   </si>
   <si>
-    <t>{'RB1', 'CDK7', 'AKT1', 'PML', 'SIRT1', 'TFDP1', 'FOXO1', 'FOXO3', 'E2F1', 'ERCC2', 'CDKN1A', 'CDKN2B', 'TP53', 'CDKN2A', 'BRCA1', 'NCOR2'}</t>
+    <t>{'TP53', 'AKT1', 'CDKN1A', 'RB1', 'CDKN2B', 'FOXO3', 'BRCA1', 'ERCC2', 'CDKN2A', 'CDK7', 'PML', 'NCOR2', 'TFDP1', 'E2F1', 'FOXO1', 'SIRT1'}</t>
   </si>
   <si>
     <t>{'CDKN2A'}</t>
@@ -153,28 +153,28 @@
     <t>{'MAML2', 'E2F5'}</t>
   </si>
   <si>
-    <t>{'FOXO1', 'FOXO3', 'TEAD1', 'TBX5', 'MAML2', 'ERLEC1', 'WWTR1', 'AMOTL2', 'ELK3', 'RBPJ', 'APH1B', 'ARHGAP26', 'CDH10', 'ZFPM2', 'UBE2J1', 'AMOT', 'THRB', 'ESR1', 'AR'}</t>
-  </si>
-  <si>
-    <t>{'GTF3C1', 'BRF1', 'CDKN2D', 'KAT2A', 'VDR', 'RXRB', 'EGR2', 'GTF2H4', 'DAXX', 'HDAC10'}</t>
-  </si>
-  <si>
-    <t>{'MAML2', 'NOTCH2', 'YAP1', 'EGFR', 'SOX9', 'PKN3', 'SIRT1', 'CBFB', 'STAT3', 'CDKN1A', 'SMAD1', 'CDK2', 'BOC', 'CDKN2A'}</t>
-  </si>
-  <si>
-    <t>{'GTF2H1', 'SMAD3', 'THRB', 'SMARCA2', 'RXRB', 'CCND2', 'CTNNB1', 'RANGAP1', 'SRC'}</t>
-  </si>
-  <si>
-    <t>{'SMAD4', 'RBPJ', 'SNW1', 'CREBBP', 'ADAM10', 'SIRT1', 'FOXO1', 'SUMO2', 'PIK3R1', 'FOXO3', 'CDKN1A', 'CTNNA1', 'CCNT1'}</t>
-  </si>
-  <si>
-    <t>{'AR', 'PML', 'CDK2', 'CDKN2C', 'HIVEP3'}</t>
-  </si>
-  <si>
-    <t>{'CDKN2A', 'MAF', 'CCNH', 'SEL1L'}</t>
-  </si>
-  <si>
-    <t>{'SMARCA4', 'ELK1', 'MED12', 'TGIF1', 'SMARCB1', 'SMARCC2', 'KDM1A', 'CTNNB1', 'TP53', 'JUP', 'VGLL4'}</t>
+    <t>{'THRB', 'CDH10', 'TBX5', 'AMOT', 'TEAD1', 'ELK3', 'APH1B', 'MAML2', 'RBPJ', 'FOXO3', 'ARHGAP26', 'ZFPM2', 'ERLEC1', 'WWTR1', 'FOXO1', 'AMOTL2', 'AR', 'ESR1', 'UBE2J1'}</t>
+  </si>
+  <si>
+    <t>{'GTF2H4', 'DAXX', 'EGR2', 'VDR', 'RXRB', 'CDKN2D', 'KAT2A', 'GTF3C1', 'BRF1', 'HDAC10'}</t>
+  </si>
+  <si>
+    <t>{'EGFR', 'CBFB', 'CDKN1A', 'CDK2', 'BOC', 'PKN3', 'NOTCH2', 'SMAD1', 'SOX9', 'CDKN2A', 'STAT3', 'MAML2', 'SIRT1', 'YAP1'}</t>
+  </si>
+  <si>
+    <t>{'RANGAP1', 'THRB', 'SRC', 'GTF2H1', 'CTNNB1', 'RXRB', 'SMARCA2', 'CCND2', 'SMAD3'}</t>
+  </si>
+  <si>
+    <t>{'RBPJ', 'CDKN1A', 'FOXO3', 'SNW1', 'CCNT1', 'PIK3R1', 'CTNNA1', 'SUMO2', 'ADAM10', 'FOXO1', 'SIRT1', 'SMAD4', 'CREBBP'}</t>
+  </si>
+  <si>
+    <t>{'AR', 'CDK2', 'CDKN2C', 'HIVEP3', 'PML'}</t>
+  </si>
+  <si>
+    <t>{'SEL1L', 'MAF', 'CDKN2A', 'CCNH'}</t>
+  </si>
+  <si>
+    <t>{'TP53', 'JUP', 'KDM1A', 'MED12', 'SMARCC2', 'SMARCB1', 'CTNNB1', 'ELK1', 'SMARCA4', 'TGIF1', 'VGLL4'}</t>
   </si>
   <si>
     <t>['ERCC2']</t>
@@ -186,37 +186,37 @@
     <t>cluster_5</t>
   </si>
   <si>
-    <t>{'CDC42', 'HRAS', 'IGF1R', 'ELN', 'INSR', 'HTRA2', 'IRS1', 'SHC1', 'PIK3CB'}</t>
-  </si>
-  <si>
-    <t>{'PAPSS2', 'RET', 'PDGFB', 'SYTL3'}</t>
-  </si>
-  <si>
-    <t>{'FBLN2', 'CR2', 'MS4A1', 'PYCR1'}</t>
-  </si>
-  <si>
-    <t>{'RCN1', 'COL5A2', 'AOX1', 'LOX', 'PIK3R3', 'PTK2', 'GPX7', 'EDN3', 'PDGFRA', 'CYCS', 'PDGFRB', 'IRS1', 'CERS6', 'CYS1', 'EMILIN1', 'KIF5B', 'THBS1', 'FYN', 'DLC1', 'RPGRIP1L', 'ITGA1', 'C3', 'UACA', 'MFAP5', 'ADAMTS2', 'ABL2', 'LTBP1', 'SIRPA', 'CXCL12', 'JAM3', 'HSP90AA1', 'RHOA', 'FBN1', 'ELN', 'RHOJ', 'SH3KBP1', 'ITGA9', 'MSR1', 'WIPF1', 'MFAP4', 'GPX8', 'ESR1', 'ANKS6', 'NRP1', 'GALNT12', 'TGFBR1', 'FBLN5', 'DOCK4', 'RHOQ', 'ITGAV', 'PIK3AP1'}</t>
-  </si>
-  <si>
-    <t>{'ITGB7', 'GRB7', 'SEMA4D', 'MOGS', 'DVL2', 'EPHB3', 'PLK1', 'COL2A1', 'CNKSR1', 'PLEKHH3', 'GJB6', 'PIK3R2', 'PSAT1', 'TROAP', 'COCH', 'PLXNB1', 'HGS', 'ADAM15'}</t>
-  </si>
-  <si>
-    <t>{'HGF', 'SERPINA1', 'LCP2', 'CD2AP', 'P4HA1', 'FGG', 'EGFR', 'FYN', 'PKN3', 'TGFB1', 'C3', 'RAB27A', 'PAPSS2', 'LTBP1', 'ITSN1', 'LRP4', 'ITGB1', 'RANBP3L', 'FCGR1A', 'CD44', 'MSR1', 'SHC1', 'TLN1', 'FLT1', 'PARD3', 'TGFB3', 'CD81', 'SYK', 'TGFBR1', 'SPP1', 'DOCK4', 'ITGB5', 'PXN', 'RHOQ', 'ECE1', 'ITGAV', 'PIK3AP1'}</t>
-  </si>
-  <si>
-    <t>{'SOS1', 'MET', 'DLG2', 'SRC', 'PIK3CB', 'DOCK3', 'F11R', 'DLG1', 'CTNNB1', 'EPHA5', 'YWHAB', 'CHRNA7', 'GOPC', 'AGPAT1', 'MYO5A', 'RCN2', 'AKAP10', 'DLGAP1', 'SMAD3'}</t>
-  </si>
-  <si>
-    <t>{'SLC44A2', 'YWHAZ', 'LRCH3', 'KRAS', 'XIAP', 'COL4A3', 'SMARCA5', 'COL4A5', 'PIK3R1', 'EIF4H', 'YWHAB'}</t>
-  </si>
-  <si>
-    <t>{'AGPAT1', 'PARD6A', 'PDGFB', 'VEGFC', 'ALKBH7', 'EML4'}</t>
-  </si>
-  <si>
-    <t>{'MFAP4', 'MYO5A', 'YWHAZ', 'GPX8', 'MITF', 'KITLG', 'DLC1', 'EML1', 'XIAP', 'RHOQ', 'OSTF1', 'TFRC'}</t>
-  </si>
-  <si>
-    <t>{'EPHB4', 'MED12', 'PARD6G', 'UNC119B', 'AGRN', 'CTNNB1', 'DVL2', 'GTF2IRD1', 'PLXNB1', 'SHC1', 'ITGA3'}</t>
+    <t>{'IRS1', 'IGF1R', 'PIK3CB', 'INSR', 'SHC1', 'ELN', 'CDC42', 'HRAS', 'HTRA2'}</t>
+  </si>
+  <si>
+    <t>{'PAPSS2', 'PDGFB', 'RET', 'SYTL3'}</t>
+  </si>
+  <si>
+    <t>{'CR2', 'FBLN2', 'MS4A1', 'PYCR1'}</t>
+  </si>
+  <si>
+    <t>{'CYS1', 'PDGFRA', 'LOX', 'ABL2', 'MFAP5', 'DOCK4', 'PIK3AP1', 'PTK2', 'GALNT12', 'SIRPA', 'EMILIN1', 'GPX8', 'NRP1', 'RHOA', 'SH3KBP1', 'MSR1', 'ELN', 'HSP90AA1', 'ITGAV', 'DLC1', 'PIK3R3', 'FBN1', 'ADAMTS2', 'KIF5B', 'C3', 'EDN3', 'WIPF1', 'AOX1', 'RHOQ', 'RCN1', 'FYN', 'UACA', 'ANKS6', 'PDGFRB', 'MFAP4', 'CYCS', 'CERS6', 'FBLN5', 'ITGA1', 'ITGA9', 'RHOJ', 'GPX7', 'RPGRIP1L', 'COL5A2', 'IRS1', 'THBS1', 'JAM3', 'ESR1', 'LTBP1', 'TGFBR1', 'CXCL12'}</t>
+  </si>
+  <si>
+    <t>{'PLXNB1', 'SEMA4D', 'DVL2', 'COL2A1', 'PIK3R2', 'PSAT1', 'PLEKHH3', 'PLK1', 'GJB6', 'CNKSR1', 'TROAP', 'ITGB7', 'COCH', 'MOGS', 'ADAM15', 'GRB7', 'HGS', 'EPHB3'}</t>
+  </si>
+  <si>
+    <t>{'TGFB3', 'ITSN1', 'SPP1', 'PKN3', 'DOCK4', 'PIK3AP1', 'RAB27A', 'HGF', 'TGFB1', 'TLN1', 'ITGB1', 'FCGR1A', 'MSR1', 'SHC1', 'ITGB5', 'ITGAV', 'PAPSS2', 'PXN', 'LRP4', 'EGFR', 'ECE1', 'C3', 'RHOQ', 'SYK', 'FYN', 'CD2AP', 'RANBP3L', 'P4HA1', 'CD81', 'FGG', 'PARD3', 'LTBP1', 'CD44', 'TGFBR1', 'SERPINA1', 'LCP2', 'FLT1'}</t>
+  </si>
+  <si>
+    <t>{'SOS1', 'MYO5A', 'GOPC', 'AGPAT1', 'CHRNA7', 'DLGAP1', 'DOCK3', 'SRC', 'CTNNB1', 'EPHA5', 'AKAP10', 'DLG2', 'SMAD3', 'F11R', 'RCN2', 'DLG1', 'PIK3CB', 'YWHAB', 'MET'}</t>
+  </si>
+  <si>
+    <t>{'SMARCA5', 'YWHAB', 'YWHAZ', 'PIK3R1', 'EIF4H', 'SLC44A2', 'COL4A5', 'COL4A3', 'KRAS', 'XIAP', 'LRCH3'}</t>
+  </si>
+  <si>
+    <t>{'ALKBH7', 'PDGFB', 'VEGFC', 'PARD6A', 'EML4', 'AGPAT1'}</t>
+  </si>
+  <si>
+    <t>{'YWHAZ', 'RHOQ', 'MYO5A', 'MITF', 'TFRC', 'XIAP', 'EML1', 'MFAP4', 'KITLG', 'GPX8', 'OSTF1', 'DLC1'}</t>
+  </si>
+  <si>
+    <t>{'PLXNB1', 'AGRN', 'UNC119B', 'GTF2IRD1', 'DVL2', 'PARD6G', 'MED12', 'CTNNB1', 'ITGA3', 'SHC1', 'EPHB4'}</t>
   </si>
   <si>
     <t>['INSR', 'ELN']</t>
@@ -243,7 +243,7 @@
     <t>cluster_4</t>
   </si>
   <si>
-    <t>{'NFKBIA', 'HTT', 'HSPA1A', 'AKT1', 'FOXO3', 'IKBKB', 'TP53'}</t>
+    <t>{'TP53', 'IKBKB', 'FOXO3', 'HTT', 'HSPA1A', 'NFKBIA', 'AKT1'}</t>
   </si>
   <si>
     <t>{'FADD'}</t>
@@ -252,25 +252,25 @@
     <t>{'RHPN2'}</t>
   </si>
   <si>
-    <t>{'CD14', 'CFLAR', 'IRAK3', 'HSP90AA1', 'RAB8B', 'CASP10', 'BCL2', 'FOXO3', 'TLR4', 'FKBP5'}</t>
-  </si>
-  <si>
-    <t>{'NFKB2', 'NLRP1', 'TBC1D17', 'IKBKE', 'TAB1', 'IKBKB', 'LRSAM1'}</t>
-  </si>
-  <si>
-    <t>{'CASP1', 'NFKBIA', 'CD14', 'BCL2L11', 'TNIP2', 'TNFRSF1B', 'RELA', 'SHMT1', 'SFN', 'BCL2', 'LTBR', 'MCL1', 'FKBP5', 'TLR4', 'TNFRSF1A', 'MAP3K8', 'MYD88'}</t>
-  </si>
-  <si>
-    <t>{'HSPH1', 'BAD', 'SARM1'}</t>
-  </si>
-  <si>
-    <t>{'CUL4A', 'CREBBP', 'FOXO3'}</t>
+    <t>{'FOXO3', 'CASP10', 'RAB8B', 'CFLAR', 'IRAK3', 'CD14', 'TLR4', 'HSP90AA1', 'BCL2', 'FKBP5'}</t>
+  </si>
+  <si>
+    <t>{'IKBKB', 'TBC1D17', 'NLRP1', 'TAB1', 'NFKB2', 'IKBKE', 'LRSAM1'}</t>
+  </si>
+  <si>
+    <t>{'TNFRSF1B', 'RELA', 'MCL1', 'MAP3K8', 'BCL2L11', 'MYD88', 'LTBR', 'SHMT1', 'CD14', 'TNIP2', 'TLR4', 'CASP1', 'BCL2', 'NFKBIA', 'FKBP5', 'SFN', 'TNFRSF1A'}</t>
+  </si>
+  <si>
+    <t>{'SARM1', 'HSPH1', 'BAD'}</t>
+  </si>
+  <si>
+    <t>{'CREBBP', 'FOXO3', 'CUL4A'}</t>
   </si>
   <si>
     <t>{'TICAM2'}</t>
   </si>
   <si>
-    <t>{'CFLAR', 'CASP10', 'TLR4', 'IRAK3'}</t>
+    <t>{'IRAK3', 'CFLAR', 'TLR4', 'CASP10'}</t>
   </si>
   <si>
     <t>{'SHMT2', 'TP53', 'FADD', 'TRAF2'}</t>
@@ -279,37 +279,37 @@
     <t>cluster_2</t>
   </si>
   <si>
-    <t>{'RB1', 'CDK7', 'AKT1', 'TFDP1', 'FOXO1', 'MYC', 'FOXO3', 'E2F1', 'CDKN1A', 'CDKN2B', 'TP53', 'ERCC8', 'CDKN2A'}</t>
+    <t>{'TP53', 'AKT1', 'MYC', 'CDKN1A', 'RB1', 'CDKN2B', 'FOXO3', 'ERCC8', 'CDKN2A', 'CDK7', 'TFDP1', 'FOXO1', 'E2F1'}</t>
   </si>
   <si>
     <t>{'DDB2', 'CDKN2A', 'SYTL3'}</t>
   </si>
   <si>
-    <t>{'E2F5', 'SUZ12'}</t>
-  </si>
-  <si>
-    <t>{'NQO1', 'AR', 'ESR1', 'KIF5B', 'FOXO1', 'FOXO3', 'YAF2'}</t>
-  </si>
-  <si>
-    <t>{'KCTD15', 'CDKN2D', 'MCM7'}</t>
-  </si>
-  <si>
-    <t>{'GMNN', 'STAT3', 'CDKN1A', 'SMAD1', 'RAB27A', 'CDK2', 'CDKN2A'}</t>
-  </si>
-  <si>
-    <t>{'MYO5A', 'MCM4', 'OAZ2', 'YY1', 'CDC6', 'KCTD1', 'CCND2', 'CTNNB1', 'SMAD3', 'YAF2'}</t>
-  </si>
-  <si>
-    <t>{'SMAD4', 'PHC3', 'YY1', 'CREBBP', 'CUL4A', 'FOXO1', 'FOXO3', 'EPC1', 'CDKN1A', 'EHMT1'}</t>
-  </si>
-  <si>
-    <t>{'AR', 'CDK2', 'CDKN2C', 'CITED4'}</t>
-  </si>
-  <si>
-    <t>{'MYO5A', 'CCNH', 'CDKN2A'}</t>
-  </si>
-  <si>
-    <t>{'EHMT2', 'PHC1', 'SMARCA4', 'TGIF1', 'KDM1A', 'CTNNB1', 'TP53', 'CITED4'}</t>
+    <t>{'SUZ12', 'E2F5'}</t>
+  </si>
+  <si>
+    <t>{'AR', 'FOXO3', 'KIF5B', 'ESR1', 'YAF2', 'NQO1', 'FOXO1'}</t>
+  </si>
+  <si>
+    <t>{'CDKN2D', 'MCM7', 'KCTD15'}</t>
+  </si>
+  <si>
+    <t>{'GMNN', 'CDKN1A', 'CDK2', 'SMAD1', 'CDKN2A', 'RAB27A', 'STAT3'}</t>
+  </si>
+  <si>
+    <t>{'CDC6', 'MCM4', 'OAZ2', 'CTNNB1', 'MYO5A', 'YY1', 'YAF2', 'KCTD1', 'CCND2', 'SMAD3'}</t>
+  </si>
+  <si>
+    <t>{'CDKN1A', 'FOXO3', 'EHMT1', 'EPC1', 'YY1', 'PHC3', 'CUL4A', 'FOXO1', 'SMAD4', 'CREBBP'}</t>
+  </si>
+  <si>
+    <t>{'AR', 'CDKN2C', 'CDK2', 'CITED4'}</t>
+  </si>
+  <si>
+    <t>{'MYO5A', 'CDKN2A', 'CCNH'}</t>
+  </si>
+  <si>
+    <t>{'TP53', 'KDM1A', 'CTNNB1', 'SMARCA4', 'TGIF1', 'PHC1', 'EHMT2', 'CITED4'}</t>
   </si>
   <si>
     <t>['ERCC8']</t>
@@ -330,31 +330,31 @@
     <t>{'HTT'}</t>
   </si>
   <si>
-    <t>{'NT5E', 'CHML', 'PAWR'}</t>
-  </si>
-  <si>
-    <t>{'RABEP1', 'OSBPL1A', 'RAB32', 'RAB8B', 'ABCD2', 'APH1B', 'SALL1', 'PEX19', 'PTP4A2', 'ARHGDIG', 'NT5E', 'PRKRA', 'LONRF3'}</t>
-  </si>
-  <si>
-    <t>{'SLC6A8', 'C19orf54', 'TMEM102', 'S1PR5', 'PPFIA3', 'TBC1D17', 'SIRT2', 'RAB38', 'GGA1'}</t>
-  </si>
-  <si>
-    <t>{'SLC6A8', 'TRIM4', 'RAB34', 'ZFP36', 'USP3', 'RAB13', 'PAWR', 'RAB31'}</t>
-  </si>
-  <si>
-    <t>{'RAB35', 'CHM', 'RAB14', 'RABEP1', 'OSBPL1A', 'ABCD2', 'VAMP2', 'TMEM9', 'BACE1', 'PRKRA', 'RAB1A'}</t>
-  </si>
-  <si>
-    <t>{'DICER1', 'CHM', 'RAB10', 'ZFP36', 'PRKRA'}</t>
-  </si>
-  <si>
-    <t>{'GGA3', 'TMEM9', 'C19orf54', 'EHD3'}</t>
-  </si>
-  <si>
-    <t>{'NT5E', 'RAB3GAP1', 'RAB31'}</t>
-  </si>
-  <si>
-    <t>{'MICALL1', 'TMEM102', 'PPFIA3'}</t>
+    <t>{'PAWR', 'NT5E', 'CHML'}</t>
+  </si>
+  <si>
+    <t>{'RABEP1', 'SALL1', 'RAB8B', 'RAB32', 'ARHGDIG', 'NT5E', 'PEX19', 'LONRF3', 'PTP4A2', 'APH1B', 'PRKRA', 'OSBPL1A', 'ABCD2'}</t>
+  </si>
+  <si>
+    <t>{'SIRT2', 'TBC1D17', 'PPFIA3', 'S1PR5', 'SLC6A8', 'TMEM102', 'GGA1', 'C19orf54', 'RAB38'}</t>
+  </si>
+  <si>
+    <t>{'PAWR', 'TRIM4', 'SLC6A8', 'RAB31', 'RAB13', 'ZFP36', 'RAB34', 'USP3'}</t>
+  </si>
+  <si>
+    <t>{'RABEP1', 'RAB1A', 'RAB14', 'TMEM9', 'BACE1', 'RAB35', 'VAMP2', 'PRKRA', 'OSBPL1A', 'ABCD2', 'CHM'}</t>
+  </si>
+  <si>
+    <t>{'ZFP36', 'DICER1', 'RAB10', 'PRKRA', 'CHM'}</t>
+  </si>
+  <si>
+    <t>{'EHD3', 'GGA3', 'C19orf54', 'TMEM9'}</t>
+  </si>
+  <si>
+    <t>{'RAB31', 'NT5E', 'RAB3GAP1'}</t>
+  </si>
+  <si>
+    <t>{'MICALL1', 'PPFIA3', 'TMEM102'}</t>
   </si>
   <si>
     <t>['RAB3GAP1']</t>

</xml_diff>